<commit_message>
set controller registration, forgotpassword, admin
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>No</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>Validation email, null(required)</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Manage user regist with all condition</t>
+  </si>
+  <si>
+    <t>Forgot Password</t>
+  </si>
+  <si>
+    <t>Manage user password with all condition</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -161,7 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -179,21 +194,126 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -480,18 +600,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="11" customWidth="1"/>
-    <col min="3" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -504,7 +625,7 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -512,68 +633,110 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -581,297 +744,29 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="D9" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>20</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>21</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>22</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>23</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>24</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>25</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>26</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>27</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>28</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>29</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="4">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F32" s="5"/>
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D31:D35">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="D10:D14">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -884,16 +779,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D30">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+  <conditionalFormatting sqref="D4:D9">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="lessThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="2" operator="lessThan">
+    <cfRule type="cellIs" priority="9" operator="lessThan">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
@@ -910,7 +811,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D31:D35</xm:sqref>
+          <xm:sqref>D10:D14</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
set controller manage user, edit view change password, edit view user/index
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -213,7 +213,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -261,56 +261,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -602,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -692,7 +642,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -780,15 +730,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D9">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>100</formula>
     </cfRule>
     <cfRule type="cellIs" priority="8" operator="lessThan">

</xml_diff>

<commit_message>
set admin Controller, security index controller, update db
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="BackEnd" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>No</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Manage User Role</t>
+  </si>
+  <si>
+    <t>Change Access</t>
+  </si>
+  <si>
+    <t>Manage Menu</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -190,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,8 +221,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -326,12 +344,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -362,7 +389,6 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -396,12 +422,287 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -941,18 +1242,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="9" customWidth="1"/>
     <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="31" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1100,14 +1401,99 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="5"/>
     </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="30">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33">
+        <f>AVERAGE(D2:D14)</f>
+        <v>0.60769230769230775</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D10:D14">
-    <cfRule type="dataBar" priority="11">
+  <mergeCells count="1">
+    <mergeCell ref="A15:C15"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1121,21 +1507,68 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D9">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="22" operator="equal">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+  <conditionalFormatting sqref="D1:D9 D14 D16:D1048576">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="19" operator="equal">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="lessThan">
+    <cfRule type="cellIs" priority="20" operator="lessThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="lessThan">
+    <cfRule type="cellIs" priority="21" operator="lessThan">
+      <formula>40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D12">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
+      <formula>0%</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D12">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="lessThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="lessThan">
+      <formula>40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{492C005C-6F75-48CE-B517-CC36857713D0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="lessThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="lessThan">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1152,7 +1585,18 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D10:D14</xm:sqref>
+          <xm:sqref>D14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{492C005C-6F75-48CE-B517-CC36857713D0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D13</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1164,7 +1608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -1175,587 +1619,587 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
-      <c r="L2" s="13" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="L2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="15"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="14"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="20"/>
-      <c r="L3" s="16" t="s">
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="19"/>
+      <c r="L3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="19" t="s">
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="21"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="17" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="20"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="21"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="19"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="20"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="20"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="17" t="str">
+      <c r="D6" s="16" t="str">
         <f>B3</f>
         <v>Title</v>
       </c>
-      <c r="E6" s="17" t="str">
+      <c r="E6" s="16" t="str">
         <f>B3</f>
         <v>Title</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="17" t="str">
+      <c r="I6" s="16" t="str">
         <f>G3</f>
         <v>Genre</v>
       </c>
-      <c r="J6" s="20" t="str">
+      <c r="J6" s="19" t="str">
         <f>G3</f>
         <v>Genre</v>
       </c>
-      <c r="L6" s="22"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="20"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="21"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="20"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="20"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="20"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="21"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="19"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="20"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="17" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="20"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="21"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="19"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="20"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="17" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="19" t="s">
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="17" t="s">
+      <c r="R10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="21"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="20"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="17" t="str">
+      <c r="D11" s="16" t="str">
         <f>B8</f>
         <v>Sheet</v>
       </c>
-      <c r="E11" s="17" t="str">
+      <c r="E11" s="16" t="str">
         <f>B8</f>
         <v>Sheet</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17" t="s">
+      <c r="F11" s="17"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="17" t="str">
+      <c r="I11" s="16" t="str">
         <f>G8</f>
         <v>Author</v>
       </c>
-      <c r="J11" s="20" t="str">
+      <c r="J11" s="19" t="str">
         <f>G8</f>
         <v>Author</v>
       </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="20"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="20"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="19"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="20"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="20"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="21"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="19"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="20"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="17" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="20"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="21"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="19"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="20"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="17" t="s">
+      <c r="F15" s="17"/>
+      <c r="G15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L15" s="23"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="21"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="20"/>
     </row>
     <row r="16" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="24"/>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="25" t="str">
+      <c r="D16" s="24" t="str">
         <f>B13</f>
         <v>Publisher</v>
       </c>
-      <c r="E16" s="25" t="str">
+      <c r="E16" s="24" t="str">
         <f>B13</f>
         <v>Publisher</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25" t="s">
+      <c r="F16" s="25"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="25" t="str">
+      <c r="I16" s="24" t="str">
         <f>G13</f>
         <v>Image</v>
       </c>
-      <c r="J16" s="27" t="str">
+      <c r="J16" s="26" t="str">
         <f>G13</f>
         <v>Image</v>
       </c>
-      <c r="L16" s="23"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="21"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="20"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="L17" s="16" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="L17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="17" t="s">
+      <c r="M17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="19" t="s">
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="R17" s="17" t="s">
+      <c r="R17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="21"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="20"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="21"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="20"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="21"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="20"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="21"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="20"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="L21" s="23"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="21"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="20"/>
     </row>
     <row r="22" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L22" s="28"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="29"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="28"/>
     </row>
     <row r="23" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L23" s="28"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="29"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="28"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="K27" t="s">

</xml_diff>